<commit_message>
Added possibility to import speed dial numbers The LDAP query part is not yet implemented
</commit_message>
<xml_diff>
--- a/ldap-server/db/testdata.xlsx
+++ b/ldap-server/db/testdata.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Github\inno-thinyldap\ldap-server\db\"/>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entreprise!$A$1:$L$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entreprise!$A$1:$N$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Tabelle1!$A$1:$F$51</definedName>
     <definedName name="oben" localSheetId="0">Entreprise!$D$3</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="249">
   <si>
     <t>Adresses partenaires / sous-traitants</t>
   </si>
@@ -759,6 +759,24 @@
   </si>
   <si>
     <t>André Schild</t>
+  </si>
+  <si>
+    <t>KurzwahlTel</t>
+  </si>
+  <si>
+    <t>KurzwahlMobile</t>
+  </si>
+  <si>
+    <t>3333</t>
+  </si>
+  <si>
+    <t>+41 79 632 07 54</t>
+  </si>
+  <si>
+    <t>3334</t>
+  </si>
+  <si>
+    <t>a.schild@aarboard.ch</t>
   </si>
 </sst>
 </file>
@@ -829,7 +847,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -854,6 +872,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1174,11 +1195,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O246"/>
+  <dimension ref="A1:Q246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1188,19 +1209,21 @@
     <col min="3" max="3" width="24.85546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="33.140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="6"/>
-    <col min="14" max="15" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="6"/>
+    <col min="6" max="6" width="23.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="6" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="6"/>
+    <col min="16" max="17" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>239</v>
       </c>
@@ -1217,28 +1240,34 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>241</v>
       </c>
@@ -1249,25 +1278,35 @@
       <c r="E2" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="F2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="12" t="s">
+        <v>248</v>
+      </c>
       <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G5" s="7"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1275,25 +1314,29 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1301,137 +1344,158 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K19" s="8"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M19" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I31" s="7"/>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.2">
       <c r="E40" s="7"/>
-      <c r="G40" s="7"/>
+      <c r="F40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-    </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="58" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E58" s="6"/>
-      <c r="G58" s="6"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F58" s="6"/>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="9"/>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J74" s="7"/>
-    </row>
-    <row r="98" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L74" s="7"/>
+    </row>
+    <row r="98" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
-    </row>
-    <row r="100" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+    </row>
+    <row r="100" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E100" s="6"/>
-      <c r="G100" s="6"/>
-    </row>
-    <row r="147" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="F100" s="6"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="147" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C147" s="8"/>
     </row>
-    <row r="157" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
-      <c r="G157" s="7"/>
+      <c r="F157" s="7"/>
       <c r="I157" s="7"/>
-      <c r="J157" s="7"/>
-    </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I182" s="7"/>
-    </row>
-    <row r="217" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="I217" s="7"/>
-    </row>
-    <row r="218" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="I218" s="7"/>
-    </row>
-    <row r="224" spans="6:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="F224"/>
-    </row>
-    <row r="241" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K157" s="7"/>
+      <c r="L157" s="7"/>
+    </row>
+    <row r="182" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K182" s="7"/>
+    </row>
+    <row r="217" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="K217" s="7"/>
+    </row>
+    <row r="218" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="K218" s="7"/>
+    </row>
+    <row r="224" spans="7:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="G224"/>
+      <c r="H224"/>
+    </row>
+    <row r="241" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B241" s="10"/>
     </row>
-    <row r="246" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="H246" s="11"/>
+    <row r="246" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="J246" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L20">
-    <sortState ref="A2:L270">
+  <autoFilter ref="A1:N20">
+    <sortState ref="A2:N270">
       <sortCondition ref="B1:B20"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="20" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="20" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added option to show exsting data
</commit_message>
<xml_diff>
--- a/ldap-server/db/testdata.xlsx
+++ b/ldap-server/db/testdata.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="256">
   <si>
     <t>Adresses partenaires / sous-traitants</t>
   </si>
@@ -777,6 +777,27 @@
   </si>
   <si>
     <t>+4179123456</t>
+  </si>
+  <si>
+    <t>Firma 2</t>
+  </si>
+  <si>
+    <t>Person 2</t>
+  </si>
+  <si>
+    <t>+41 32 332 97 15</t>
+  </si>
+  <si>
+    <t>3335</t>
+  </si>
+  <si>
+    <t>+4179123457</t>
+  </si>
+  <si>
+    <t>3336</t>
+  </si>
+  <si>
+    <t>hier@aarboard.ch</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1220,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1295,7 +1316,28 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
@@ -1493,9 +1535,10 @@
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="20" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="20" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2588,18 +2631,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2621,6 +2664,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D86F47A-5D79-4152-9F57-B9FE87555AAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558457C1-FC0E-4F99-83EF-A803456498F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="60e93e53-976b-4b74-a2df-28443208662f"/>
@@ -2634,12 +2685,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D86F47A-5D79-4152-9F57-B9FE87555AAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added a lot of other fields, like home, zip, city etc. Improved Innovaphone DECT handling
</commit_message>
<xml_diff>
--- a/ldap-server/db/testdata.xlsx
+++ b/ldap-server/db/testdata.xlsx
@@ -12,11 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Entreprise" sheetId="2" r:id="rId1"/>
+    <sheet name="Phonebook" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entreprise!$A$1:$N$20</definedName>
-    <definedName name="oben" localSheetId="0">Entreprise!$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Phonebook!$A$1:$O$20</definedName>
+    <definedName name="oben" localSheetId="0">Phonebook!$C$3</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateCount="2000"/>
   <extLst>
@@ -28,59 +28,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Entreprise</t>
-  </si>
-  <si>
-    <t>Personne</t>
-  </si>
-  <si>
-    <t>Fonction</t>
-  </si>
-  <si>
-    <t>Tel</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>E-Mail</t>
   </si>
   <si>
-    <t>Adresse</t>
-  </si>
-  <si>
     <t>Fax</t>
   </si>
   <si>
-    <t>Ville</t>
-  </si>
-  <si>
-    <t>Pays</t>
-  </si>
-  <si>
-    <t>Case Postale</t>
-  </si>
-  <si>
     <t>Mobile</t>
   </si>
   <si>
-    <t>Etat</t>
-  </si>
-  <si>
     <t>+41 32 332 97 14</t>
   </si>
   <si>
     <t>Aarboard AG</t>
   </si>
   <si>
-    <t>André Schild</t>
-  </si>
-  <si>
-    <t>KurzwahlTel</t>
-  </si>
-  <si>
-    <t>KurzwahlMobile</t>
-  </si>
-  <si>
     <t>3333</t>
   </si>
   <si>
@@ -112,6 +76,60 @@
   </si>
   <si>
     <t>hier@aarboard.ch</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Schild</t>
+  </si>
+  <si>
+    <t>André</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>KW Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Egliweg 10</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Nidau</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>KW Mobile</t>
+  </si>
+  <si>
+    <t>+41323329715</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>KW Home</t>
   </si>
 </sst>
 </file>
@@ -189,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -206,9 +224,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -217,6 +232,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -536,326 +563,347 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q246"/>
+  <dimension ref="A1:R246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="4"/>
-    <col min="2" max="2" width="27.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="4" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="4"/>
-    <col min="16" max="17" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" style="4" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="4"/>
+    <col min="17" max="18" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2560</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I5" s="8"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
-      <c r="J7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O9" s="5"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M19" s="5"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K31" s="8"/>
-    </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-    </row>
-    <row r="58" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="N38" s="7"/>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="N40" s="7"/>
+    </row>
+    <row r="58" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H58" s="4"/>
       <c r="I58" s="4"/>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B69" s="9"/>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="L74" s="8"/>
-    </row>
-    <row r="98" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="N58" s="4"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="8"/>
+    </row>
+    <row r="98" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
-    </row>
-    <row r="100" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+    </row>
+    <row r="100" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H100" s="4"/>
       <c r="I100" s="4"/>
-    </row>
-    <row r="147" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C147" s="5"/>
-    </row>
-    <row r="157" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D157" s="8"/>
-      <c r="E157" s="8"/>
-      <c r="F157" s="8"/>
-      <c r="I157" s="8"/>
-      <c r="K157" s="8"/>
-      <c r="L157" s="8"/>
-    </row>
-    <row r="182" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K182" s="8"/>
-    </row>
-    <row r="217" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="K217" s="8"/>
-    </row>
-    <row r="218" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="K218" s="8"/>
-    </row>
-    <row r="224" spans="7:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="G224" s="10"/>
-      <c r="H224" s="10"/>
-    </row>
-    <row r="241" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B241" s="11"/>
-    </row>
-    <row r="246" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="J246" s="7"/>
+      <c r="N100" s="4"/>
+    </row>
+    <row r="147" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B147" s="5"/>
+    </row>
+    <row r="157" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C157" s="7"/>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
+      <c r="F157" s="7"/>
+      <c r="G157" s="7"/>
+      <c r="H157" s="7"/>
+      <c r="I157" s="7"/>
+      <c r="N157" s="7"/>
+    </row>
+    <row r="224" spans="10:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="J224" s="9"/>
+      <c r="K224" s="9"/>
+      <c r="L224" s="9"/>
+      <c r="M224" s="9"/>
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A241" s="10"/>
+    </row>
+    <row r="246" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="O246" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N20">
-    <sortState ref="A2:N270">
-      <sortCondition ref="B1:B20"/>
-    </sortState>
-  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="20" orientation="portrait" r:id="rId3"/>
@@ -863,18 +911,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1018,6 +1066,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D86F47A-5D79-4152-9F57-B9FE87555AAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558457C1-FC0E-4F99-83EF-A803456498F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="60e93e53-976b-4b74-a2df-28443208662f"/>
@@ -1029,14 +1085,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D86F47A-5D79-4152-9F57-B9FE87555AAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>